<commit_message>
update before session 2
</commit_message>
<xml_diff>
--- a/COEN R Sessions/R Workshop (Responses).xlsx
+++ b/COEN R Sessions/R Workshop (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="25">
   <si>
     <t>Timestamp</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>I wish to gain sufficient proficiency in R to start to use it instead of SPSS for the next analysis I'll be taking on at work</t>
+  </si>
+  <si>
+    <t>Become proficient in using R for small scale projects</t>
+  </si>
+  <si>
+    <t>To gain more R knowledge so I can better utilize it at work!</t>
   </si>
 </sst>
 </file>
@@ -635,6 +641,70 @@
         <v>22</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>44263.43841596065</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>44264.416566423606</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>